<commit_message>
update the gps tracing
</commit_message>
<xml_diff>
--- a/report/file.xlsx
+++ b/report/file.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,115 +424,15 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2024-01-01 00:00:00</v>
-      </c>
-      <c r="B2">
-        <v>0.00021</v>
-      </c>
-      <c r="C2">
-        <v>0.23</v>
+        <v>2024-10-25 02:38:09</v>
       </c>
       <c r="D2" t="str">
-        <v>2024-10-24 15:54:57</v>
-      </c>
-      <c r="E2">
-        <v>0.000231</v>
-      </c>
-      <c r="F2">
-        <v>0.902923</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2024-10-24 15:55:40</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2024-10-24 15:56:46</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2024-10-24 15:58:05</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2024-10-24 15:59:44</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2024-10-24 16:01:51</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2024-10-24 16:04:15</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2024-10-24 16:44:59</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2024-10-24 16:45:06</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>2024-10-24 16:48:10</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2024-10-24 16:48:12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>2024-10-24 16:48:16</v>
-      </c>
-      <c r="D8" t="str">
-        <v>2024-10-24 16:48:21</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>2024-10-24 16:48:51</v>
-      </c>
-      <c r="D9" t="str">
-        <v>2024-10-24 16:55:06</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>2024-10-24 16:55:13</v>
-      </c>
-      <c r="D10" t="str">
-        <v>2024-10-24 20:18:45</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>2024-10-24 20:18:52</v>
-      </c>
-      <c r="D11" t="str">
-        <v>2024-10-24 20:18:55</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>2024-10-24 20:19:08</v>
-      </c>
-      <c r="D12" t="str">
-        <v>2024-10-24 20:19:11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>2024-10-24 20:19:13</v>
-      </c>
-      <c r="D13" t="str">
-        <v>2024-10-24 20:19:22</v>
+        <v>2024-10-25 02:38:25</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
file downlaod with serverless function
</commit_message>
<xml_diff>
--- a/report/file.xlsx
+++ b/report/file.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,17 +422,9 @@
         <v>Longitud</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2024-10-25 02:38:09</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-10-25 02:38:25</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>